<commit_message>
updated webservice queries and added one graph
</commit_message>
<xml_diff>
--- a/graphs/langugageDistributionGraph.xlsx
+++ b/graphs/langugageDistributionGraph.xlsx
@@ -999,12 +999,24 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400" b="1"/>
-                  <a:t>Count of languages</a:t>
+                  <a:t>Number</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+                  <a:t> of different projects using Language</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.8205128205128206E-2"/>
+              <c:y val="9.3084444444444442E-2"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1958,7 +1970,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>